<commit_message>
1.Developed a new test in catalog module - CancelRequisiton_RecentOrdersList. 2. Added a new method in Requisitioning page - cancelRequisitionFromRecentOrders(String comments).
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/AddPriceAgreement_LocalCatalog.xlsx
+++ b/src/test/resources/datasheets/AddPriceAgreement_LocalCatalog.xlsx
@@ -374,12 +374,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>